<commit_message>
Tablas de estadisticas parte A y B de sim3 netlogo
</commit_message>
<xml_diff>
--- a/Tarea4/parte2/sim3Netlogo/analisis_resultados.xlsx
+++ b/Tarea4/parte2/sim3Netlogo/analisis_resultados.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spere\Documents\repo_modsim\ModSimGrp6\Tarea4\parte2\sim3Netlogo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09516169-B378-4763-B3FD-D5E07BA88732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91B09D-4718-4A33-97E1-1ED1F0984ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analisis Parte A" sheetId="2" r:id="rId1"/>
     <sheet name="Analisis Parte B" sheetId="5" r:id="rId2"/>
-    <sheet name="simulacion3 ParteA-table" sheetId="3" r:id="rId3"/>
-    <sheet name="simulacion3 ParteB-table" sheetId="4" r:id="rId4"/>
-    <sheet name="ruta documento" sheetId="1" r:id="rId5"/>
+    <sheet name="Analisis Parte C" sheetId="6" r:id="rId3"/>
+    <sheet name="simulacion3 ParteA-table" sheetId="3" r:id="rId4"/>
+    <sheet name="simulacion3 ParteB-table" sheetId="4" r:id="rId5"/>
+    <sheet name="ruta documento" sheetId="1" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="2" hidden="1">'simulacion3 ParteA-table'!$A$1:$H$51</definedName>
-    <definedName name="DatosExternos_1" localSheetId="3" hidden="1">'simulacion3 ParteB-table'!$A$1:$H$51</definedName>
+    <definedName name="DatosExternos_1" localSheetId="3" hidden="1">'simulacion3 ParteA-table'!$A$1:$H$51</definedName>
+    <definedName name="DatosExternos_1" localSheetId="4" hidden="1">'simulacion3 ParteB-table'!$A$1:$H$51</definedName>
+    <definedName name="Estadisticas_A">'Analisis Parte A'!$A$1:$E$6</definedName>
+    <definedName name="Estadisticas_B">'Analisis Parte B'!$A$1:$E$6</definedName>
     <definedName name="Ruta">'ruta documento'!$A$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId6"/>
-    <pivotCache cacheId="23" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId7"/>
+    <pivotCache cacheId="9" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -82,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="25">
   <si>
     <t>[run number]</t>
   </si>
@@ -117,14 +120,53 @@
     <t>Total general</t>
   </si>
   <si>
-    <t>Promedio de death-percentage</t>
+    <t>Num Ambulancias</t>
+  </si>
+  <si>
+    <t>Num Hospitales</t>
+  </si>
+  <si>
+    <t>Promedio % Muertes</t>
+  </si>
+  <si>
+    <t>Desviación Estándar</t>
+  </si>
+  <si>
+    <t>Muestra</t>
+  </si>
+  <si>
+    <t>Error IC 95%</t>
+  </si>
+  <si>
+    <t>Experimento</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Promedio Max Cm</t>
+  </si>
+  <si>
+    <t>Promedio de max-patient-counter</t>
+  </si>
+  <si>
+    <t>Datos A</t>
+  </si>
+  <si>
+    <t>Datos B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,16 +174,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -149,20 +242,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -185,7 +386,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="spere" refreshedDate="45496.755641435186" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="50" xr:uid="{09C3770F-21A9-4D2B-865B-145CBEAFB052}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="spere" refreshedDate="45496.783525231484" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="50" xr:uid="{57611DC7-9B3A-49E6-862C-17B524E23FB5}">
   <cacheSource type="worksheet">
     <worksheetSource name="Datos_A"/>
   </cacheSource>
@@ -230,7 +431,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="spere" refreshedDate="45496.756167013889" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="50" xr:uid="{60AE4F79-F957-42C9-8E2D-6372D1C96CE9}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="spere" refreshedDate="45496.784049884256" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="50" xr:uid="{F9A6415E-495A-4525-90F7-3E6AA19E0945}">
   <cacheSource type="worksheet">
     <worksheetSource name="Datos_B"/>
   </cacheSource>
@@ -1285,8 +1486,71 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{842C6F11-B550-47FA-8F9B-F6D40E285F32}" name="TablaDinámica3" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FB4E855E-3B50-4746-B3F6-1BDFAF95A495}" name="TablaDinámica2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="D13:E19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Promedio de max-patient-counter" fld="7" subtotal="average" baseField="2" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{356578AC-FCF1-497A-83A9-0BC6BF351335}" name="TablaDinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A13:B19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -1303,8 +1567,8 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="3"/>
@@ -1333,70 +1597,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Promedio de death-percentage" fld="6" subtotal="average" baseField="3" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4ECCA2DB-CD2F-4F68-844C-F732A236B6B3}" name="TablaDinámica4" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="2"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Promedio de death-percentage" fld="6" subtotal="average" baseField="2" baseItem="0"/>
+    <dataField name="Promedio de max-patient-counter" fld="7" subtotal="average" baseField="3" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1741,70 +1942,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC12663-D3D3-4197-9B67-8D8D10A47459}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" cm="1">
+        <f t="array" ref="A2:A6">_xlfn.UNIQUE(Datos_A[num-ambulances])</f>
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
+        <f>AVERAGEIF(Datos_A[num-ambulances],A2,Datos_A[death-percentage])</f>
         <v>59.356999999999992</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="C2" s="6" cm="1">
+        <f t="array" ref="C2">_xlfn.STDEV.S(IF(Datos_A[num-ambulances]=A2,Datos_A[death-percentage]))</f>
+        <v>1.4471278066877455</v>
+      </c>
+      <c r="D2" s="6">
+        <f>COUNTIF(Datos_A[num-ambulances],A2)</f>
+        <v>10</v>
+      </c>
+      <c r="E2" s="6">
+        <f>_xlfn.CONFIDENCE.T(0.05,C2,D2)</f>
+        <v>1.03521287033626</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="8">
+        <f>AVERAGEIF(Datos_A[num-ambulances],A3,Datos_A[death-percentage])</f>
         <v>29.216999999999995</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="C3" s="8" cm="1">
+        <f t="array" ref="C3">_xlfn.STDEV.S(IF(Datos_A[num-ambulances]=A3,Datos_A[death-percentage]))</f>
+        <v>1.9830450770917381</v>
+      </c>
+      <c r="D3" s="8">
+        <f>COUNTIF(Datos_A[num-ambulances],A3)</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E6" si="0">_xlfn.CONFIDENCE.T(0.05,C3,D3)</f>
+        <v>1.4185849907487043</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="6">
+        <f>AVERAGEIF(Datos_A[num-ambulances],A4,Datos_A[death-percentage])</f>
         <v>10.259</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="C4" s="6" cm="1">
+        <f t="array" ref="C4">_xlfn.STDEV.S(IF(Datos_A[num-ambulances]=A4,Datos_A[death-percentage]))</f>
+        <v>2.0094745028931804</v>
+      </c>
+      <c r="D4" s="6">
+        <f>COUNTIF(Datos_A[num-ambulances],A4)</f>
+        <v>10</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4374914630166054</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="8">
+        <f>AVERAGEIF(Datos_A[num-ambulances],A5,Datos_A[death-percentage])</f>
         <v>1.2549999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="C5" s="8" cm="1">
+        <f t="array" ref="C5">_xlfn.STDEV.S(IF(Datos_A[num-ambulances]=A5,Datos_A[death-percentage]))</f>
+        <v>0.77162526886796245</v>
+      </c>
+      <c r="D5" s="8">
+        <f>COUNTIF(Datos_A[num-ambulances],A5)</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.55198746490616801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <f>AVERAGEIF(Datos_A[num-ambulances],A6,Datos_A[death-percentage])</f>
         <v>0.01</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="6" cm="1">
+        <f t="array" ref="C6">_xlfn.STDEV.S(IF(Datos_A[num-ambulances]=A6,Datos_A[death-percentage]))</f>
+        <v>1.4142135623730951E-2</v>
+      </c>
+      <c r="D6" s="6">
+        <f>COUNTIF(Datos_A[num-ambulances],A6)</f>
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>20.019600000000001</v>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>1.011667438360969E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1814,70 +2087,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C62862D3-6BFE-4BB5-8A09-C0582253F6E2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" cm="1">
+        <f t="array" ref="A2:A6">_xlfn.UNIQUE(Datos_B[num-hospitals])</f>
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="13">
+        <f>AVERAGEIF(Datos_B[num-hospitals],A2,Datos_B[death-percentage])</f>
         <v>59.064999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="C2" s="13" cm="1">
+        <f t="array" ref="C2">_xlfn.STDEV.S(IF(Datos_B[num-hospitals]=A2,Datos_B[death-percentage]))</f>
+        <v>3.4901201825852488</v>
+      </c>
+      <c r="D2" s="13">
+        <f>COUNTIF(Datos_B[num-hospitals],A2)</f>
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <f>_xlfn.CONFIDENCE.T(0.05,C2,D2)</f>
+        <v>2.4966815752799549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="15">
+        <f>AVERAGEIF(Datos_B[num-hospitals],A3,Datos_B[death-percentage])</f>
         <v>28.417999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="C3" s="15" cm="1">
+        <f t="array" ref="C3">_xlfn.STDEV.S(IF(Datos_B[num-hospitals]=A3,Datos_B[death-percentage]))</f>
+        <v>2.3033974906646053</v>
+      </c>
+      <c r="D3" s="15">
+        <f>COUNTIF(Datos_B[num-hospitals],A3)</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="15">
+        <f t="shared" ref="E3:E6" si="0">_xlfn.CONFIDENCE.T(0.05,C3,D3)</f>
+        <v>1.6477513021424253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="13">
+        <f>AVERAGEIF(Datos_B[num-hospitals],A4,Datos_B[death-percentage])</f>
         <v>9.5149999999999988</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="C4" s="13" cm="1">
+        <f t="array" ref="C4">_xlfn.STDEV.S(IF(Datos_B[num-hospitals]=A4,Datos_B[death-percentage]))</f>
+        <v>1.4082159714412468</v>
+      </c>
+      <c r="D4" s="13">
+        <f>COUNTIF(Datos_B[num-hospitals],A4)</f>
+        <v>10</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>1.0073770202686843</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="15">
+        <f>AVERAGEIF(Datos_B[num-hospitals],A5,Datos_B[death-percentage])</f>
         <v>1.2270000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="C5" s="15" cm="1">
+        <f t="array" ref="C5">_xlfn.STDEV.S(IF(Datos_B[num-hospitals]=A5,Datos_B[death-percentage]))</f>
+        <v>0.86797401394793428</v>
+      </c>
+      <c r="D5" s="15">
+        <f>COUNTIF(Datos_B[num-hospitals],A5)</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.62091120508073294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13">
+        <f>AVERAGEIF(Datos_B[num-hospitals],A6,Datos_B[death-percentage])</f>
         <v>1.5999999999999997E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="C6" s="13" cm="1">
+        <f t="array" ref="C6">_xlfn.STDEV.S(IF(Datos_B[num-hospitals]=A6,Datos_B[death-percentage]))</f>
+        <v>2.0655911179772894E-2</v>
+      </c>
+      <c r="D6" s="13">
+        <f>COUNTIF(Datos_B[num-hospitals],A6)</f>
         <v>10</v>
       </c>
-      <c r="B7" s="1">
-        <v>19.648200000000003</v>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>1.4776348711567203E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1886,11 +2230,258 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB64BAA-E6DD-4788-9728-23F73DE33BC3}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="24">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>451.8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1989.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="9">
+        <v>827.2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1952.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1151.7</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1839.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>4</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1523.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1820.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>5</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1703.4</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1789.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9">
+        <v>1131.52</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1878.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4529ED-88B7-46B2-81BC-2918DFE27098}">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1944,7 +2535,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2">
@@ -1970,7 +2561,7 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3">
@@ -1996,7 +2587,7 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4">
@@ -2022,7 +2613,7 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5">
@@ -2048,7 +2639,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6">
@@ -2074,7 +2665,7 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7">
@@ -2100,7 +2691,7 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8">
@@ -2126,7 +2717,7 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9">
@@ -2152,7 +2743,7 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10">
@@ -2178,7 +2769,7 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11">
@@ -2204,7 +2795,7 @@
       <c r="D12">
         <v>2</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12">
@@ -2230,7 +2821,7 @@
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
@@ -2256,7 +2847,7 @@
       <c r="D14">
         <v>2</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14">
@@ -2282,7 +2873,7 @@
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15">
@@ -2308,7 +2899,7 @@
       <c r="D16">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16">
@@ -2334,7 +2925,7 @@
       <c r="D17">
         <v>2</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17">
@@ -2360,7 +2951,7 @@
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18">
@@ -2386,7 +2977,7 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19">
@@ -2412,7 +3003,7 @@
       <c r="D20">
         <v>2</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="F20">
@@ -2438,7 +3029,7 @@
       <c r="D21">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
@@ -2464,7 +3055,7 @@
       <c r="D22">
         <v>3</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22">
@@ -2490,7 +3081,7 @@
       <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23">
@@ -2516,7 +3107,7 @@
       <c r="D24">
         <v>3</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24">
@@ -2542,7 +3133,7 @@
       <c r="D25">
         <v>3</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>8</v>
       </c>
       <c r="F25">
@@ -2568,7 +3159,7 @@
       <c r="D26">
         <v>3</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>8</v>
       </c>
       <c r="F26">
@@ -2594,7 +3185,7 @@
       <c r="D27">
         <v>3</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
       <c r="F27">
@@ -2620,7 +3211,7 @@
       <c r="D28">
         <v>3</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>8</v>
       </c>
       <c r="F28">
@@ -2646,7 +3237,7 @@
       <c r="D29">
         <v>3</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>8</v>
       </c>
       <c r="F29">
@@ -2672,7 +3263,7 @@
       <c r="D30">
         <v>4</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>8</v>
       </c>
       <c r="F30">
@@ -2698,7 +3289,7 @@
       <c r="D31">
         <v>3</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>8</v>
       </c>
       <c r="F31">
@@ -2724,7 +3315,7 @@
       <c r="D32">
         <v>4</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>8</v>
       </c>
       <c r="F32">
@@ -2750,7 +3341,7 @@
       <c r="D33">
         <v>4</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>8</v>
       </c>
       <c r="F33">
@@ -2776,7 +3367,7 @@
       <c r="D34">
         <v>3</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>8</v>
       </c>
       <c r="F34">
@@ -2802,7 +3393,7 @@
       <c r="D35">
         <v>4</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>8</v>
       </c>
       <c r="F35">
@@ -2828,7 +3419,7 @@
       <c r="D36">
         <v>4</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>8</v>
       </c>
       <c r="F36">
@@ -2854,7 +3445,7 @@
       <c r="D37">
         <v>4</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37">
@@ -2880,7 +3471,7 @@
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38">
@@ -2906,7 +3497,7 @@
       <c r="D39">
         <v>5</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>8</v>
       </c>
       <c r="F39">
@@ -2932,7 +3523,7 @@
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>8</v>
       </c>
       <c r="F40">
@@ -2958,7 +3549,7 @@
       <c r="D41">
         <v>5</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>8</v>
       </c>
       <c r="F41">
@@ -2984,7 +3575,7 @@
       <c r="D42">
         <v>4</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>8</v>
       </c>
       <c r="F42">
@@ -3010,7 +3601,7 @@
       <c r="D43">
         <v>4</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>8</v>
       </c>
       <c r="F43">
@@ -3036,7 +3627,7 @@
       <c r="D44">
         <v>5</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>8</v>
       </c>
       <c r="F44">
@@ -3062,7 +3653,7 @@
       <c r="D45">
         <v>5</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>8</v>
       </c>
       <c r="F45">
@@ -3088,7 +3679,7 @@
       <c r="D46">
         <v>5</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>8</v>
       </c>
       <c r="F46">
@@ -3114,7 +3705,7 @@
       <c r="D47">
         <v>5</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>8</v>
       </c>
       <c r="F47">
@@ -3140,7 +3731,7 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>8</v>
       </c>
       <c r="F48">
@@ -3166,7 +3757,7 @@
       <c r="D49">
         <v>5</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>8</v>
       </c>
       <c r="F49">
@@ -3192,7 +3783,7 @@
       <c r="D50">
         <v>5</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>8</v>
       </c>
       <c r="F50">
@@ -3218,7 +3809,7 @@
       <c r="D51">
         <v>5</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>8</v>
       </c>
       <c r="F51">
@@ -3239,12 +3830,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A11BC3-3F1D-4C65-8FC3-7BA1672CA2CD}">
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3298,7 +3889,7 @@
       <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2">
@@ -3324,7 +3915,7 @@
       <c r="D3">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3">
@@ -3350,7 +3941,7 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4">
@@ -3376,7 +3967,7 @@
       <c r="D5">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5">
@@ -3402,7 +3993,7 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6">
@@ -3428,7 +4019,7 @@
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7">
@@ -3454,7 +4045,7 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8">
@@ -3480,7 +4071,7 @@
       <c r="D9">
         <v>5</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9">
@@ -3506,7 +4097,7 @@
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10">
@@ -3532,7 +4123,7 @@
       <c r="D11">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11">
@@ -3558,7 +4149,7 @@
       <c r="D12">
         <v>5</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12">
@@ -3584,7 +4175,7 @@
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
@@ -3610,7 +4201,7 @@
       <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14">
@@ -3636,7 +4227,7 @@
       <c r="D15">
         <v>5</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15">
@@ -3662,7 +4253,7 @@
       <c r="D16">
         <v>5</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16">
@@ -3688,7 +4279,7 @@
       <c r="D17">
         <v>5</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17">
@@ -3714,7 +4305,7 @@
       <c r="D18">
         <v>5</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18">
@@ -3740,7 +4331,7 @@
       <c r="D19">
         <v>5</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19">
@@ -3766,7 +4357,7 @@
       <c r="D20">
         <v>5</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="F20">
@@ -3792,7 +4383,7 @@
       <c r="D21">
         <v>5</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
@@ -3818,7 +4409,7 @@
       <c r="D22">
         <v>5</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22">
@@ -3844,7 +4435,7 @@
       <c r="D23">
         <v>5</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23">
@@ -3870,7 +4461,7 @@
       <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>8</v>
       </c>
       <c r="F24">
@@ -3896,7 +4487,7 @@
       <c r="D25">
         <v>5</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>8</v>
       </c>
       <c r="F25">
@@ -3922,7 +4513,7 @@
       <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>8</v>
       </c>
       <c r="F26">
@@ -3948,7 +4539,7 @@
       <c r="D27">
         <v>5</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
       <c r="F27">
@@ -3974,7 +4565,7 @@
       <c r="D28">
         <v>5</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>8</v>
       </c>
       <c r="F28">
@@ -4000,7 +4591,7 @@
       <c r="D29">
         <v>5</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>8</v>
       </c>
       <c r="F29">
@@ -4026,7 +4617,7 @@
       <c r="D30">
         <v>5</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>8</v>
       </c>
       <c r="F30">
@@ -4052,7 +4643,7 @@
       <c r="D31">
         <v>5</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>8</v>
       </c>
       <c r="F31">
@@ -4078,7 +4669,7 @@
       <c r="D32">
         <v>5</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>8</v>
       </c>
       <c r="F32">
@@ -4104,7 +4695,7 @@
       <c r="D33">
         <v>5</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>8</v>
       </c>
       <c r="F33">
@@ -4130,7 +4721,7 @@
       <c r="D34">
         <v>5</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>8</v>
       </c>
       <c r="F34">
@@ -4156,7 +4747,7 @@
       <c r="D35">
         <v>5</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>8</v>
       </c>
       <c r="F35">
@@ -4182,7 +4773,7 @@
       <c r="D36">
         <v>5</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>8</v>
       </c>
       <c r="F36">
@@ -4208,7 +4799,7 @@
       <c r="D37">
         <v>5</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>8</v>
       </c>
       <c r="F37">
@@ -4234,7 +4825,7 @@
       <c r="D38">
         <v>5</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>8</v>
       </c>
       <c r="F38">
@@ -4260,7 +4851,7 @@
       <c r="D39">
         <v>5</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>8</v>
       </c>
       <c r="F39">
@@ -4286,7 +4877,7 @@
       <c r="D40">
         <v>5</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>8</v>
       </c>
       <c r="F40">
@@ -4312,7 +4903,7 @@
       <c r="D41">
         <v>5</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>8</v>
       </c>
       <c r="F41">
@@ -4338,7 +4929,7 @@
       <c r="D42">
         <v>5</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>8</v>
       </c>
       <c r="F42">
@@ -4364,7 +4955,7 @@
       <c r="D43">
         <v>5</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>8</v>
       </c>
       <c r="F43">
@@ -4390,7 +4981,7 @@
       <c r="D44">
         <v>5</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>8</v>
       </c>
       <c r="F44">
@@ -4416,7 +5007,7 @@
       <c r="D45">
         <v>5</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>8</v>
       </c>
       <c r="F45">
@@ -4442,7 +5033,7 @@
       <c r="D46">
         <v>5</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>8</v>
       </c>
       <c r="F46">
@@ -4468,7 +5059,7 @@
       <c r="D47">
         <v>5</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>8</v>
       </c>
       <c r="F47">
@@ -4494,7 +5085,7 @@
       <c r="D48">
         <v>5</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>8</v>
       </c>
       <c r="F48">
@@ -4520,7 +5111,7 @@
       <c r="D49">
         <v>5</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>8</v>
       </c>
       <c r="F49">
@@ -4546,7 +5137,7 @@
       <c r="D50">
         <v>5</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>8</v>
       </c>
       <c r="F50">
@@ -4572,7 +5163,7 @@
       <c r="D51">
         <v>5</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>8</v>
       </c>
       <c r="F51">
@@ -4593,7 +5184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>